<commit_message>
don't affect first two header rows
</commit_message>
<xml_diff>
--- a/excel.xlsx
+++ b/excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SamirHabota\Desktop\Export\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A80AF8A1-BF3D-4D86-8107-54C62968E72F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01C5D18F-37EA-43A5-ACF2-177758B4FD11}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="5" xr2:uid="{F0F4F4C8-6F96-4880-A933-1B38950B8945}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{F0F4F4C8-6F96-4880-A933-1B38950B8945}"/>
   </bookViews>
   <sheets>
     <sheet name="Iman Siručić" sheetId="12" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1225" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1225" uniqueCount="44">
   <si>
     <t>MAIN INFO</t>
   </si>
@@ -166,6 +166,9 @@
   </si>
   <si>
     <t>Bonus4/Dodano za jul Marku</t>
+  </si>
+  <si>
+    <t>Samir</t>
   </si>
 </sst>
 </file>
@@ -553,15 +556,6 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -573,6 +567,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -890,8 +893,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF57BF86-57DE-4294-B07D-CA205991B1E3}">
   <dimension ref="A1:U149"/>
   <sheetViews>
-    <sheetView topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -899,7 +902,7 @@
     <row r="1" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="32" t="s">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="C1" s="33"/>
       <c r="D1" s="34"/>
@@ -922,14 +925,14 @@
       </c>
       <c r="P1" s="42"/>
       <c r="Q1" s="43"/>
-      <c r="R1" s="47" t="s">
+      <c r="R1" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="S1" s="48"/>
-      <c r="T1" s="49" t="s">
+      <c r="S1" s="45"/>
+      <c r="T1" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="U1" s="50"/>
+      <c r="U1" s="47"/>
     </row>
     <row r="2" spans="1:21" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4"/>
@@ -7249,12 +7252,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="T1:U1"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:I1"/>
     <mergeCell ref="J1:N1"/>
     <mergeCell ref="O1:Q1"/>
     <mergeCell ref="R1:S1"/>
-    <mergeCell ref="T1:U1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7296,14 +7299,14 @@
       </c>
       <c r="P1" s="42"/>
       <c r="Q1" s="43"/>
-      <c r="R1" s="47" t="s">
+      <c r="R1" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="S1" s="48"/>
-      <c r="T1" s="49" t="s">
+      <c r="S1" s="45"/>
+      <c r="T1" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="U1" s="50"/>
+      <c r="U1" s="47"/>
     </row>
     <row r="2" spans="1:21" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4"/>
@@ -13631,12 +13634,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="T1:U1"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:I1"/>
     <mergeCell ref="J1:N1"/>
     <mergeCell ref="O1:Q1"/>
     <mergeCell ref="R1:S1"/>
-    <mergeCell ref="T1:U1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -13678,14 +13681,14 @@
       </c>
       <c r="P1" s="42"/>
       <c r="Q1" s="43"/>
-      <c r="R1" s="47" t="s">
+      <c r="R1" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="S1" s="48"/>
-      <c r="T1" s="49" t="s">
+      <c r="S1" s="45"/>
+      <c r="T1" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="U1" s="50"/>
+      <c r="U1" s="47"/>
     </row>
     <row r="2" spans="1:21" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4"/>
@@ -19965,12 +19968,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="T1:U1"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:I1"/>
     <mergeCell ref="J1:N1"/>
     <mergeCell ref="O1:Q1"/>
     <mergeCell ref="R1:S1"/>
-    <mergeCell ref="T1:U1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -20012,14 +20015,14 @@
       </c>
       <c r="P1" s="42"/>
       <c r="Q1" s="43"/>
-      <c r="R1" s="47" t="s">
+      <c r="R1" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="S1" s="48"/>
-      <c r="T1" s="49" t="s">
+      <c r="S1" s="45"/>
+      <c r="T1" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="U1" s="50"/>
+      <c r="U1" s="47"/>
     </row>
     <row r="2" spans="1:21" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4"/>
@@ -26325,12 +26328,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="T1:U1"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:I1"/>
     <mergeCell ref="J1:N1"/>
     <mergeCell ref="O1:Q1"/>
     <mergeCell ref="R1:S1"/>
-    <mergeCell ref="T1:U1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -26372,14 +26375,14 @@
       </c>
       <c r="P1" s="42"/>
       <c r="Q1" s="43"/>
-      <c r="R1" s="47" t="s">
+      <c r="R1" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="S1" s="48"/>
-      <c r="T1" s="49" t="s">
+      <c r="S1" s="45"/>
+      <c r="T1" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="U1" s="50"/>
+      <c r="U1" s="47"/>
     </row>
     <row r="2" spans="1:21" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4"/>
@@ -32699,12 +32702,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="T1:U1"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:I1"/>
     <mergeCell ref="J1:N1"/>
     <mergeCell ref="O1:Q1"/>
     <mergeCell ref="R1:S1"/>
-    <mergeCell ref="T1:U1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -32714,7 +32717,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{533B1E12-3841-4D6C-872E-81D0BD84CE28}">
   <dimension ref="A1:AI986"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="T147" sqref="T147:U147"/>
     </sheetView>
   </sheetViews>
@@ -41981,24 +41984,24 @@
     </row>
     <row r="158" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A158" s="3"/>
-      <c r="B158" s="44"/>
-      <c r="C158" s="45"/>
-      <c r="D158" s="45"/>
-      <c r="E158" s="46"/>
-      <c r="F158" s="44"/>
-      <c r="G158" s="45"/>
-      <c r="H158" s="45"/>
-      <c r="I158" s="46"/>
+      <c r="B158" s="48"/>
+      <c r="C158" s="49"/>
+      <c r="D158" s="49"/>
+      <c r="E158" s="50"/>
+      <c r="F158" s="48"/>
+      <c r="G158" s="49"/>
+      <c r="H158" s="49"/>
+      <c r="I158" s="50"/>
       <c r="J158" s="3"/>
-      <c r="K158" s="44"/>
-      <c r="L158" s="45"/>
-      <c r="M158" s="45"/>
-      <c r="N158" s="45"/>
-      <c r="O158" s="46"/>
-      <c r="P158" s="44"/>
-      <c r="Q158" s="45"/>
-      <c r="R158" s="45"/>
-      <c r="S158" s="46"/>
+      <c r="K158" s="48"/>
+      <c r="L158" s="49"/>
+      <c r="M158" s="49"/>
+      <c r="N158" s="49"/>
+      <c r="O158" s="50"/>
+      <c r="P158" s="48"/>
+      <c r="Q158" s="49"/>
+      <c r="R158" s="49"/>
+      <c r="S158" s="50"/>
       <c r="T158" s="3"/>
       <c r="U158" s="3"/>
       <c r="V158" s="3"/>
@@ -72704,14 +72707,14 @@
       </c>
       <c r="P1" s="42"/>
       <c r="Q1" s="43"/>
-      <c r="R1" s="47" t="s">
+      <c r="R1" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="S1" s="48"/>
-      <c r="T1" s="49" t="s">
+      <c r="S1" s="45"/>
+      <c r="T1" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="U1" s="50"/>
+      <c r="U1" s="47"/>
     </row>
     <row r="2" spans="1:21" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4"/>

</xml_diff>